<commit_message>
Updated the datasheets for OAK-SoM, OAK-SoM-IoT and OAK-SoM-Pro Updated IO table for OAK-SoM-Pro
</commit_message>
<xml_diff>
--- a/SoMs/OAK-SoM-Pro/OAK-SoM-Pro_IO_TABLE.xlsx
+++ b/SoMs/OAK-SoM-Pro/OAK-SoM-Pro_IO_TABLE.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="330">
   <si>
     <t>Pin #</t>
   </si>
@@ -678,9 +678,6 @@
     <t>JTAG</t>
   </si>
   <si>
-    <t>SDS signal</t>
-  </si>
-  <si>
     <t>Camera D I2C SDA (if applicable). Can be used as GPIO</t>
   </si>
   <si>
@@ -714,9 +711,6 @@
     <t xml:space="preserve">Should be pulled low with PD: 10kR/GND. Any SGPIO pin can be used to wake up the SoM. </t>
   </si>
   <si>
-    <t>GPIO_37_3V3</t>
-  </si>
-  <si>
     <t>GPIO_37</t>
   </si>
   <si>
@@ -918,34 +912,123 @@
     <t>2099EMB INTERFACE CONNECTOR B</t>
   </si>
   <si>
-    <t>GPIO_8/SPI0_CS_1</t>
-  </si>
-  <si>
-    <t>GPIO_36_3V3</t>
-  </si>
-  <si>
-    <t>GPIO_35_3V3</t>
-  </si>
-  <si>
-    <t>GPIO_34_3V3</t>
-  </si>
-  <si>
-    <t>GPIO_32_3V3</t>
-  </si>
-  <si>
-    <t>GPIO_33_3V3</t>
+    <t>MXIO_36_3V3</t>
+  </si>
+  <si>
+    <t>MXIO_37_3V3</t>
+  </si>
+  <si>
+    <t>MXIO_35_3V3</t>
+  </si>
+  <si>
+    <t>MXIO_34_3V3</t>
+  </si>
+  <si>
+    <t>MXIO_7</t>
+  </si>
+  <si>
+    <t>MXIO_32_3V3</t>
+  </si>
+  <si>
+    <t>MXIO_33_3V3</t>
+  </si>
+  <si>
+    <t>MXIO_53</t>
+  </si>
+  <si>
+    <t>MXIO_8/SPI0_CS_1</t>
+  </si>
+  <si>
+    <t>MXIO_46</t>
+  </si>
+  <si>
+    <t>MXIO_45</t>
+  </si>
+  <si>
+    <t>MXIO_6</t>
+  </si>
+  <si>
+    <t>MXIO_9</t>
+  </si>
+  <si>
+    <t>MXIO_10</t>
+  </si>
+  <si>
+    <t>MXIO_11</t>
+  </si>
+  <si>
+    <t>MXIO_12</t>
+  </si>
+  <si>
+    <t>MXIO_14</t>
+  </si>
+  <si>
+    <t>MXIO_15</t>
+  </si>
+  <si>
+    <t>MXIO_16</t>
+  </si>
+  <si>
+    <t>MXIO_17</t>
+  </si>
+  <si>
+    <t>MXIO_38</t>
+  </si>
+  <si>
+    <t>MXIO_39</t>
+  </si>
+  <si>
+    <t>MXIO_40</t>
+  </si>
+  <si>
+    <t>MXIO_42</t>
+  </si>
+  <si>
+    <t>MXIO_43</t>
+  </si>
+  <si>
+    <t>PCIe differential reference clock input from clock generator negative</t>
+  </si>
+  <si>
+    <t>PCIe differential reference clock input from clock generator positive</t>
+  </si>
+  <si>
+    <t>PCIe x1 lane transmitter data differential pair positive. Board implements AC coupling caps on board</t>
+  </si>
+  <si>
+    <t>PCIe x1 lane transmitter data differential pair negative. Board implements AC coupling caps on board</t>
+  </si>
+  <si>
+    <t>PCIe x1 lane receiver data differential pair positive</t>
+  </si>
+  <si>
+    <t>PCIe x1 lane receiver data differential pair negative</t>
+  </si>
+  <si>
+    <t>Ref Clk request Signal</t>
+  </si>
+  <si>
+    <t>PD: 10kR/1.8V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -981,6 +1064,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -999,9 +1089,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1009,11 +1101,11 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1022,13 +1114,15 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal_CONNECTOR A" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1338,11 +1432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:Y103"/>
+  <dimension ref="A1:Y175"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,7 +1451,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1402,7 +1495,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1416,7 +1509,7 @@
       </c>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1430,7 +1523,7 @@
       </c>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1446,7 +1539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1464,7 +1557,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1482,7 +1575,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1499,7 +1592,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1513,7 +1606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1527,7 +1620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1544,7 +1637,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1560,7 +1653,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1578,7 +1671,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1594,7 +1687,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1608,7 +1701,7 @@
       </c>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1622,7 +1715,7 @@
       </c>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1638,7 +1731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1654,7 +1747,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1670,7 +1763,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1686,7 +1779,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1700,7 +1793,7 @@
       </c>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1713,7 +1806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1729,7 +1822,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1745,7 +1838,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1761,7 +1854,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1777,7 +1870,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1790,7 +1883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1803,7 +1896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1827,7 +1920,7 @@
         <v>43</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>44</v>
@@ -1839,7 +1932,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1855,7 +1948,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1870,7 +1963,7 @@
       <c r="P32" s="1"/>
       <c r="Y32" s="2"/>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1883,15 +1976,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>231</v>
+        <v>298</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D34" t="s">
         <v>48</v>
@@ -1923,10 +2016,10 @@
         <v>54</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>55</v>
@@ -1949,7 +2042,7 @@
         <v>58</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -1969,10 +2062,10 @@
         <v>60</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E37" s="6"/>
       <c r="H37" s="4" t="s">
@@ -1985,15 +2078,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D38" t="s">
         <v>62</v>
@@ -2030,15 +2123,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D40" t="s">
         <v>68</v>
@@ -2078,15 +2171,15 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D42" t="s">
         <v>73</v>
@@ -2124,7 +2217,7 @@
         <v>72</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2135,7 +2228,7 @@
         <v>78</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -2147,7 +2240,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2160,7 +2253,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2172,7 +2265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2185,7 +2278,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2200,7 +2293,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2213,7 +2306,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2228,7 +2321,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2241,7 +2334,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2253,7 +2346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2266,7 +2359,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2279,7 +2372,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2292,7 +2385,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2305,7 +2398,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2318,7 +2411,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2331,7 +2424,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2344,7 +2437,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2364,10 +2457,10 @@
         <v>59</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>242</v>
+        <v>301</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -2386,10 +2479,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>83</v>
@@ -2402,15 +2495,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D63" t="s">
         <v>85</v>
@@ -2436,7 +2529,7 @@
         <v>87</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D64" s="4"/>
       <c r="H64" s="4"/>
@@ -2447,15 +2540,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D65" t="s">
         <v>89</v>
@@ -2484,7 +2577,7 @@
         <v>92</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D66" s="4"/>
       <c r="H66" s="4"/>
@@ -2503,7 +2596,7 @@
         <v>94</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1" t="s">
@@ -2521,7 +2614,7 @@
         <v>96</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D68" s="4"/>
       <c r="H68" s="4" t="s">
@@ -2542,7 +2635,7 @@
         <v>137</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D69" s="4"/>
       <c r="H69" s="4" t="s">
@@ -2563,7 +2656,7 @@
         <v>99</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>101</v>
@@ -2580,10 +2673,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>252</v>
+        <v>304</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>101</v>
@@ -2601,7 +2694,7 @@
         <v>135</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>101</v>
@@ -2613,7 +2706,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2627,7 +2720,7 @@
       </c>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2649,7 +2742,7 @@
         <v>103</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>44</v>
@@ -2669,7 +2762,7 @@
         <v>105</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H76" s="4"/>
       <c r="I76" s="1" t="s">
@@ -2679,7 +2772,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2692,7 +2785,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2713,10 +2806,10 @@
         <v>107</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H79" s="4" t="s">
         <v>56</v>
@@ -2736,7 +2829,7 @@
         <v>91</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>91</v>
@@ -2748,7 +2841,7 @@
         <v>15</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
@@ -2759,10 +2852,10 @@
         <v>109</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H81" s="4" t="s">
         <v>56</v>
@@ -2782,7 +2875,7 @@
         <v>76</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>76</v>
@@ -2794,10 +2887,10 @@
         <v>15</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2810,7 +2903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2823,7 +2916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2839,7 +2932,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2855,7 +2948,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2871,7 +2964,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2887,7 +2980,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2900,7 +2993,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2913,7 +3006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2929,7 +3022,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2945,7 +3038,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2961,7 +3054,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2977,7 +3070,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2990,7 +3083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3003,7 +3096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3019,7 +3112,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3035,7 +3128,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3051,7 +3144,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3067,7 +3160,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3080,7 +3173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3100,15 +3193,242 @@
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
     </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="5"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="5"/>
+      <c r="B105" s="4"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="5"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="5"/>
+      <c r="B107" s="4"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="5"/>
+      <c r="B108" s="4"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="5"/>
+      <c r="B109" s="4"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="5"/>
+      <c r="B110" s="4"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="5"/>
+      <c r="B111" s="4"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="5"/>
+      <c r="B112" s="4"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="5"/>
+      <c r="B113" s="4"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="5"/>
+      <c r="B115" s="4"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="5"/>
+      <c r="B116" s="4"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="5"/>
+      <c r="B117" s="4"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="5"/>
+      <c r="B118" s="4"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="5"/>
+      <c r="B119" s="4"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="5"/>
+      <c r="B120" s="4"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="5"/>
+      <c r="B121" s="4"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="5"/>
+      <c r="B122" s="4"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="5"/>
+      <c r="B123" s="4"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="5"/>
+      <c r="B124" s="4"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="5"/>
+      <c r="C126" s="4"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="5"/>
+      <c r="B127" s="4"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="5"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="5"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="5"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="5"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="5"/>
+      <c r="B133" s="4"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="5"/>
+      <c r="B134" s="4"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="5"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="5"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="5"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="5"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="5"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="5"/>
+      <c r="B142" s="4"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="5"/>
+      <c r="B143" s="4"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="5"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="5"/>
+      <c r="B145" s="4"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="5"/>
+      <c r="C146" s="4"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="5"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="5"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="5"/>
+      <c r="C150" s="4"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="5"/>
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="5"/>
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="5"/>
+      <c r="B153" s="4"/>
+      <c r="C153" s="4"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="5"/>
+      <c r="B154" s="4"/>
+      <c r="C154" s="4"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="5"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="5"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="5"/>
+      <c r="B158" s="4"/>
+      <c r="C158" s="4"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="5"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="5"/>
+      <c r="B161" s="4"/>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="5"/>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="5"/>
+      <c r="B164" s="4"/>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="5"/>
+      <c r="B165" s="4"/>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="5"/>
+      <c r="B166" s="4"/>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="5"/>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="5"/>
+      <c r="B168" s="4"/>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="5"/>
+      <c r="B170" s="4"/>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="5"/>
+      <c r="B171" s="4"/>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="5"/>
+      <c r="B172" s="4"/>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="5"/>
+      <c r="B173" s="4"/>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="5"/>
+      <c r="B174" s="4"/>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="5"/>
+      <c r="B175" s="4"/>
+    </row>
   </sheetData>
   <autoFilter ref="A2:J102">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="1.8V GPIO"/>
-        <filter val="1.8V Input"/>
-        <filter val="1.8V Output"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A30:J82">
       <sortCondition ref="A2:A102"/>
     </sortState>
@@ -3116,7 +3436,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3124,11 +3444,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:U107"/>
+  <dimension ref="A1:U164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3144,7 +3463,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3188,7 +3507,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3201,7 +3520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3214,7 +3533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3229,7 +3548,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3245,7 +3564,7 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3263,7 +3582,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3282,7 +3601,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3300,7 +3619,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3318,7 +3637,7 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3337,7 +3656,7 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3356,7 +3675,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3376,7 +3695,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3396,7 +3715,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3413,7 +3732,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3430,7 +3749,7 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -3447,7 +3766,7 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
-    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3464,18 +3783,22 @@
       <c r="U18" s="1"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>263</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="1" t="s">
-        <v>228</v>
+      <c r="I19" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>210</v>
@@ -3485,20 +3808,24 @@
       <c r="U19" s="1"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>166</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>293</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J20" t="s">
+      <c r="I20" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>205</v>
       </c>
       <c r="N20" s="1"/>
@@ -3506,197 +3833,227 @@
       <c r="U20" s="1"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>167</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>264</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
       <c r="H21" s="5"/>
-      <c r="I21" s="1" t="s">
-        <v>228</v>
+      <c r="I21" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <v>63</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>183</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>287</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="J22" t="s">
+      <c r="I22" s="5" t="s">
         <v>225</v>
       </c>
+      <c r="J22" s="4" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="5">
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>168</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="1" t="s">
-        <v>229</v>
+      <c r="I23" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="5">
         <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C24" t="s">
-        <v>265</v>
+      <c r="C24" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
-      <c r="I24" s="1" t="s">
-        <v>228</v>
+      <c r="I24" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="5">
         <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C25" t="s">
-        <v>291</v>
-      </c>
+      <c r="C25" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="1" t="s">
-        <v>229</v>
+      <c r="I25" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="5">
         <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>173</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>266</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="1" t="s">
-        <v>228</v>
+      <c r="I26" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="5">
         <v>24</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C27" t="s">
-        <v>290</v>
+      <c r="C27" s="4" t="s">
+        <v>288</v>
       </c>
       <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="1" t="s">
-        <v>229</v>
+      <c r="I27" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="5">
         <v>25</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="5" t="s">
         <v>171</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="1" t="s">
-        <v>228</v>
+      <c r="I28" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="5">
         <v>26</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="5" t="s">
         <v>174</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>289</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="1" t="s">
-        <v>229</v>
+      <c r="I29" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="5">
         <v>27</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="5" t="s">
         <v>175</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>268</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="1" t="s">
-        <v>228</v>
+      <c r="I30" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -3707,26 +4064,32 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="H31" s="5"/>
+      <c r="I31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
         <v>30</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="4"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
         <v>31</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -3737,13 +4100,13 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" t="s">
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3757,7 +4120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3782,7 +4145,7 @@
         <v>176</v>
       </c>
       <c r="C36" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D36" s="4"/>
       <c r="H36" s="5"/>
@@ -3793,7 +4156,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3819,7 +4182,7 @@
         <v>177</v>
       </c>
       <c r="C38" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D38" s="5"/>
       <c r="H38" s="4" t="s">
@@ -3832,7 +4195,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3850,7 +4213,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3862,7 +4225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3879,7 +4242,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3892,7 +4255,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3917,7 +4280,7 @@
         <v>178</v>
       </c>
       <c r="C44" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4"/>
@@ -3933,7 +4296,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3956,10 +4319,10 @@
         <v>42</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>273</v>
+        <v>306</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>13</v>
@@ -3977,7 +4340,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3994,7 +4357,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4007,7 +4370,7 @@
       </c>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4030,10 +4393,10 @@
         <v>44</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>272</v>
+        <v>307</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>18</v>
@@ -4052,7 +4415,7 @@
       </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4075,10 +4438,10 @@
         <v>48</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>274</v>
+        <v>308</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="1" t="s">
@@ -4089,7 +4452,7 @@
       </c>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>51</v>
       </c>
@@ -4113,10 +4476,10 @@
         <v>50</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="1" t="s">
@@ -4127,7 +4490,7 @@
       </c>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4151,10 +4514,10 @@
         <v>52</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>275</v>
+        <v>310</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D56" s="4"/>
       <c r="H56" s="5"/>
@@ -4166,7 +4529,7 @@
       </c>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4190,10 +4553,10 @@
         <v>54</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>276</v>
+        <v>311</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -4213,10 +4576,10 @@
         <v>56</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>277</v>
+        <v>312</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -4239,14 +4602,14 @@
         <v>181</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H60" s="4"/>
       <c r="I60" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K60" s="1"/>
     </row>
@@ -4255,10 +4618,10 @@
         <v>58</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>278</v>
+        <v>313</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -4273,7 +4636,7 @@
       </c>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>65</v>
       </c>
@@ -4281,18 +4644,20 @@
         <v>184</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="H62" s="2"/>
+        <v>294</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="I62" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J62" t="s">
-        <v>225</v>
+        <v>328</v>
       </c>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4318,7 +4683,7 @@
         <v>182</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -4329,7 +4694,7 @@
         <v>15</v>
       </c>
       <c r="J64" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -4337,10 +4702,10 @@
         <v>60</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>279</v>
+        <v>314</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -4359,10 +4724,10 @@
         <v>62</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>280</v>
+        <v>315</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="1" t="s">
@@ -4377,10 +4742,10 @@
         <v>64</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>281</v>
+        <v>316</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -4396,10 +4761,10 @@
         <v>66</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>282</v>
+        <v>317</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -4409,7 +4774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4430,10 +4795,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>283</v>
+        <v>318</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -4443,7 +4808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4456,10 +4821,10 @@
       <c r="G71" s="4"/>
       <c r="H71" s="2"/>
       <c r="I71" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J71" t="s">
-        <v>219</v>
+        <v>324</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -4467,17 +4832,17 @@
         <v>70</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>284</v>
+        <v>319</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -4487,10 +4852,10 @@
       <c r="C73" s="5"/>
       <c r="H73" s="2"/>
       <c r="I73" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J73" t="s">
-        <v>219</v>
+        <v>325</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -4498,17 +4863,17 @@
         <v>72</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>285</v>
+        <v>320</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -4526,10 +4891,10 @@
         <v>74</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>286</v>
+        <v>321</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -4540,7 +4905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -4549,13 +4914,13 @@
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J77" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -4568,7 +4933,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4577,13 +4942,13 @@
       </c>
       <c r="H79" s="4"/>
       <c r="I79" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J79" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4599,7 +4964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4611,7 +4976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4630,7 +4995,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -4641,13 +5006,13 @@
       <c r="D83" s="4"/>
       <c r="H83" s="5"/>
       <c r="I83" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J83" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4664,7 +5029,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4678,13 +5043,13 @@
       <c r="G85" s="4"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J85" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4703,7 +5068,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4716,7 +5081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4735,7 +5100,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4748,7 +5113,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4765,7 +5130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4777,15 +5142,17 @@
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
-      <c r="H91" s="1"/>
+      <c r="H91" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="I91" s="1" t="s">
         <v>218</v>
       </c>
       <c r="J91" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4804,7 +5171,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -4812,15 +5179,17 @@
         <v>198</v>
       </c>
       <c r="C93" s="1"/>
-      <c r="H93" s="1"/>
+      <c r="H93" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="I93" s="1" t="s">
         <v>218</v>
       </c>
       <c r="J93" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -4839,7 +5208,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -4850,15 +5219,17 @@
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
       <c r="G95" s="4"/>
-      <c r="H95" s="1"/>
+      <c r="H95" s="4" t="s">
+        <v>329</v>
+      </c>
       <c r="I95" s="1" t="s">
         <v>218</v>
       </c>
       <c r="J95" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -4874,7 +5245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -4885,15 +5256,17 @@
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
       <c r="G97" s="4"/>
-      <c r="H97" s="1"/>
+      <c r="H97" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="I97" s="1" t="s">
         <v>218</v>
       </c>
       <c r="J97" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -4911,7 +5284,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -4919,15 +5292,17 @@
         <v>203</v>
       </c>
       <c r="C99" s="1"/>
-      <c r="H99" s="1"/>
+      <c r="H99" s="4" t="s">
+        <v>329</v>
+      </c>
       <c r="I99" s="1" t="s">
         <v>218</v>
       </c>
       <c r="J99" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4942,7 +5317,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4950,15 +5325,17 @@
         <v>204</v>
       </c>
       <c r="C101" s="1"/>
-      <c r="H101" s="5"/>
+      <c r="H101" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="I101" s="1" t="s">
         <v>218</v>
       </c>
       <c r="J101" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4978,27 +5355,249 @@
       <c r="H103" s="5"/>
       <c r="I103" s="1"/>
     </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="5"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="5"/>
+      <c r="C105" s="4"/>
+    </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
+      <c r="C106" s="4"/>
       <c r="H106" s="5"/>
       <c r="I106" s="1"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
+      <c r="B107" s="5"/>
+      <c r="C107" s="4"/>
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
     </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="5"/>
+      <c r="B108" s="5"/>
+      <c r="C108" s="4"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="5"/>
+      <c r="B109" s="5"/>
+      <c r="C109" s="4"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="5"/>
+      <c r="B111" s="5"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="5"/>
+      <c r="B112" s="5"/>
+      <c r="C112" s="4"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="5"/>
+      <c r="B113" s="5"/>
+      <c r="C113" s="4"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="5"/>
+      <c r="B114" s="5"/>
+      <c r="C114" s="4"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="5"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="5"/>
+      <c r="B116" s="5"/>
+      <c r="C116" s="4"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="5"/>
+      <c r="B118" s="5"/>
+      <c r="C118" s="4"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="5"/>
+      <c r="B119" s="5"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="5"/>
+      <c r="B121" s="5"/>
+      <c r="C121" s="4"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="5"/>
+      <c r="B122" s="5"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="5"/>
+      <c r="B124" s="5"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="5"/>
+      <c r="B125" s="5"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="5"/>
+      <c r="B127" s="5"/>
+      <c r="C127" s="4"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="5"/>
+      <c r="B128" s="5"/>
+      <c r="C128" s="4"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="5"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="4"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="5"/>
+      <c r="B130" s="5"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="5"/>
+      <c r="B131" s="5"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="5"/>
+      <c r="B132" s="5"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="5"/>
+      <c r="B133" s="5"/>
+      <c r="C133" s="4"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="5"/>
+      <c r="B134" s="5"/>
+      <c r="C134" s="4"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="5"/>
+      <c r="B135" s="5"/>
+      <c r="C135" s="4"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="5"/>
+      <c r="B136" s="5"/>
+      <c r="C136" s="5"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="5"/>
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="5"/>
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="5"/>
+      <c r="B139" s="5"/>
+      <c r="C139" s="5"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="5"/>
+      <c r="B140" s="5"/>
+      <c r="C140" s="5"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="5"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="5"/>
+      <c r="B142" s="5"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="5"/>
+      <c r="B143" s="5"/>
+      <c r="C143" s="4"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="5"/>
+      <c r="B144" s="5"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="5"/>
+      <c r="B145" s="5"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="5"/>
+      <c r="B146" s="5"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="5"/>
+      <c r="B147" s="5"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="5"/>
+      <c r="B148" s="5"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="5"/>
+      <c r="B149" s="5"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="5"/>
+      <c r="B151" s="5"/>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="5"/>
+      <c r="B152" s="5"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="5"/>
+      <c r="B153" s="5"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="5"/>
+      <c r="B154" s="5"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="5"/>
+      <c r="B155" s="5"/>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="5"/>
+      <c r="B156" s="5"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="5"/>
+      <c r="B157" s="5"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="5"/>
+      <c r="B159" s="5"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="5"/>
+      <c r="B160" s="5"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="5"/>
+      <c r="B161" s="5"/>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="5"/>
+      <c r="B162" s="5"/>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="5"/>
+      <c r="B163" s="5"/>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="5"/>
+      <c r="B164" s="5"/>
+    </row>
   </sheetData>
   <autoFilter ref="A2:J102">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="1.8V GPIO"/>
-        <filter val="BOOT"/>
-        <filter val="I2S"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A19:J76">
       <sortCondition ref="A2:A102"/>
     </sortState>
@@ -5006,8 +5605,8 @@
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrected errors on swapped USBRX, I2C description, added voltage levels
</commit_message>
<xml_diff>
--- a/SoMs/OAK-SoM-Pro/OAK-SoM-Pro_IO_TABLE.xlsx
+++ b/SoMs/OAK-SoM-Pro/OAK-SoM-Pro_IO_TABLE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="7125" yWindow="3900" windowWidth="20805" windowHeight="14430" activeTab="1"/>
+    <workbookView xWindow="7125" yWindow="3900" windowWidth="20805" windowHeight="14430"/>
   </bookViews>
   <sheets>
     <sheet name="CONNECTOR A" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="306">
   <si>
     <t>Pin #</t>
   </si>
@@ -705,12 +705,6 @@
     <t>SDS</t>
   </si>
   <si>
-    <t>I2S</t>
-  </si>
-  <si>
-    <t>BOOT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Should be pulled low with PD: 10kR/GND. Any SGPIO pin can be used to wake up the SoM. </t>
   </si>
   <si>
@@ -934,6 +928,15 @@
   </si>
   <si>
     <t>GPIO_33_3V3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.8V I2S </t>
+  </si>
+  <si>
+    <t>1.8V BOOT</t>
+  </si>
+  <si>
+    <t>1.8V I2S</t>
   </si>
 </sst>
 </file>
@@ -1341,8 +1344,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Y103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J79" sqref="J79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,7 +1361,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1827,7 +1830,7 @@
         <v>43</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>44</v>
@@ -1888,10 +1891,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D34" t="s">
         <v>48</v>
@@ -1923,10 +1926,10 @@
         <v>54</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>55</v>
@@ -1949,7 +1952,7 @@
         <v>58</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -1969,10 +1972,10 @@
         <v>60</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E37" s="6"/>
       <c r="H37" s="4" t="s">
@@ -1990,10 +1993,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D38" t="s">
         <v>62</v>
@@ -2035,10 +2038,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D40" t="s">
         <v>68</v>
@@ -2083,10 +2086,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D42" t="s">
         <v>73</v>
@@ -2124,7 +2127,7 @@
         <v>72</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2135,7 +2138,7 @@
         <v>78</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -2364,10 +2367,10 @@
         <v>59</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -2386,10 +2389,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>83</v>
@@ -2407,10 +2410,10 @@
         <v>61</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D63" t="s">
         <v>85</v>
@@ -2436,7 +2439,7 @@
         <v>87</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D64" s="4"/>
       <c r="H64" s="4"/>
@@ -2452,10 +2455,10 @@
         <v>63</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D65" t="s">
         <v>89</v>
@@ -2484,7 +2487,7 @@
         <v>92</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D66" s="4"/>
       <c r="H66" s="4"/>
@@ -2503,7 +2506,7 @@
         <v>94</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1" t="s">
@@ -2521,7 +2524,7 @@
         <v>96</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D68" s="4"/>
       <c r="H68" s="4" t="s">
@@ -2542,7 +2545,7 @@
         <v>137</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D69" s="4"/>
       <c r="H69" s="4" t="s">
@@ -2563,7 +2566,7 @@
         <v>99</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>101</v>
@@ -2580,10 +2583,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>101</v>
@@ -2601,7 +2604,7 @@
         <v>135</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>101</v>
@@ -2649,7 +2652,7 @@
         <v>103</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>44</v>
@@ -2669,7 +2672,7 @@
         <v>105</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H76" s="4"/>
       <c r="I76" s="1" t="s">
@@ -2713,10 +2716,10 @@
         <v>107</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H79" s="4" t="s">
         <v>56</v>
@@ -2725,7 +2728,7 @@
         <v>15</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -2736,7 +2739,7 @@
         <v>91</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>91</v>
@@ -2751,7 +2754,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2759,10 +2762,10 @@
         <v>109</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H81" s="4" t="s">
         <v>56</v>
@@ -2771,10 +2774,11 @@
         <v>15</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="K81" s="4"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2782,7 +2786,7 @@
         <v>76</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>76</v>
@@ -2797,7 +2801,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2810,7 +2814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2823,7 +2827,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2839,7 +2843,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2855,7 +2859,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2871,7 +2875,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2887,7 +2891,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2900,7 +2904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2913,7 +2917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2929,7 +2933,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2945,7 +2949,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2961,7 +2965,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2977,7 +2981,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2990,7 +2994,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3127,8 +3131,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:U107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3144,7 +3148,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3463,7 +3467,7 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3471,11 +3475,11 @@
         <v>165</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="1" t="s">
-        <v>228</v>
+        <v>303</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>210</v>
@@ -3484,7 +3488,7 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3492,11 +3496,11 @@
         <v>166</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="1" t="s">
-        <v>229</v>
+        <v>304</v>
       </c>
       <c r="J20" t="s">
         <v>205</v>
@@ -3505,7 +3509,7 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -3513,11 +3517,11 @@
         <v>167</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="1" t="s">
-        <v>228</v>
+        <v>305</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>211</v>
@@ -3531,7 +3535,7 @@
         <v>183</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="1" t="s">
@@ -3541,7 +3545,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -3549,7 +3553,7 @@
         <v>168</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -3557,13 +3561,13 @@
       <c r="G23" s="4"/>
       <c r="H23" s="5"/>
       <c r="I23" s="1" t="s">
-        <v>229</v>
+        <v>304</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -3571,7 +3575,7 @@
         <v>169</v>
       </c>
       <c r="C24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -3579,13 +3583,13 @@
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
       <c r="I24" s="1" t="s">
-        <v>228</v>
+        <v>305</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -3593,17 +3597,17 @@
         <v>170</v>
       </c>
       <c r="C25" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="1" t="s">
-        <v>229</v>
+        <v>304</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -3611,17 +3615,17 @@
         <v>173</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="1" t="s">
-        <v>228</v>
+        <v>305</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -3629,18 +3633,18 @@
         <v>172</v>
       </c>
       <c r="C27" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D27" s="4"/>
       <c r="H27" s="5"/>
       <c r="I27" s="1" t="s">
-        <v>229</v>
+        <v>304</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -3648,18 +3652,18 @@
         <v>171</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D28" s="4"/>
       <c r="H28" s="5"/>
       <c r="I28" s="1" t="s">
-        <v>228</v>
+        <v>305</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -3667,17 +3671,17 @@
         <v>174</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="1" t="s">
-        <v>229</v>
+        <v>304</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -3685,11 +3689,11 @@
         <v>175</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="1" t="s">
-        <v>228</v>
+        <v>305</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>215</v>
@@ -3782,7 +3786,7 @@
         <v>176</v>
       </c>
       <c r="C36" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D36" s="4"/>
       <c r="H36" s="5"/>
@@ -3819,7 +3823,7 @@
         <v>177</v>
       </c>
       <c r="C38" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D38" s="5"/>
       <c r="H38" s="4" t="s">
@@ -3917,7 +3921,7 @@
         <v>178</v>
       </c>
       <c r="C44" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4"/>
@@ -3956,10 +3960,10 @@
         <v>42</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>13</v>
@@ -4030,10 +4034,10 @@
         <v>44</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>18</v>
@@ -4075,10 +4079,10 @@
         <v>48</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="1" t="s">
@@ -4113,10 +4117,10 @@
         <v>50</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="1" t="s">
@@ -4151,10 +4155,10 @@
         <v>52</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D56" s="4"/>
       <c r="H56" s="5"/>
@@ -4190,10 +4194,10 @@
         <v>54</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -4213,10 +4217,10 @@
         <v>56</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -4239,7 +4243,7 @@
         <v>181</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H60" s="4"/>
       <c r="I60" s="1" t="s">
@@ -4255,10 +4259,10 @@
         <v>58</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -4281,7 +4285,7 @@
         <v>184</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="1" t="s">
@@ -4318,7 +4322,7 @@
         <v>182</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -4337,10 +4341,10 @@
         <v>60</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -4359,10 +4363,10 @@
         <v>62</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="1" t="s">
@@ -4377,10 +4381,10 @@
         <v>64</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -4396,10 +4400,10 @@
         <v>66</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -4430,10 +4434,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -4467,10 +4471,10 @@
         <v>70</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="1" t="s">
@@ -4498,10 +4502,10 @@
         <v>72</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="1" t="s">
@@ -4526,10 +4530,10 @@
         <v>74</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -4684,7 +4688,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4716,7 +4720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4785,7 +4789,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4820,7 +4824,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -4893,12 +4897,12 @@
         <v>224</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -4927,12 +4931,12 @@
         <v>224</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H100" s="5"/>
       <c r="I100" s="1" t="s">
@@ -4995,8 +4999,9 @@
     <filterColumn colId="8">
       <filters>
         <filter val="1.8V GPIO"/>
-        <filter val="BOOT"/>
-        <filter val="I2S"/>
+        <filter val="USB2"/>
+        <filter val="USB3/Input"/>
+        <filter val="USB3/Output"/>
       </filters>
     </filterColumn>
     <sortState ref="A19:J76">

</xml_diff>